<commit_message>
Add Note Calculation Doc
</commit_message>
<xml_diff>
--- a/docs/Note Step Calculation.xlsx
+++ b/docs/Note Step Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suple\Desktop\escw2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8172A54D-1407-439C-A997-C84C97D8A95F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D69BF7-B52C-4AFE-90B2-0E1F0DFBDB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{AEB0162C-2A5D-4A5F-9B45-F4F039314D0D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="19">
   <si>
     <t>sampling frequency (Hz)</t>
   </si>
@@ -447,16 +447,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2415B402-AA1C-4106-B29D-C23625C3A3F9}">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="6.20703125" customWidth="1"/>
     <col min="4" max="4" width="10.62890625" customWidth="1"/>
+    <col min="6" max="6" width="13.26171875" customWidth="1"/>
     <col min="9" max="9" width="10.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -497,21 +498,21 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C10" si="0">C4/$F$1</f>
-        <v>65.406391324758047</v>
+        <f t="shared" ref="C3:C14" si="0">C4/$F$1</f>
+        <v>32.703195662117956</v>
       </c>
       <c r="D3" s="1">
-        <f>($I$1*C3)/$A$1</f>
-        <v>6370029.7435195902</v>
-      </c>
-      <c r="F3">
-        <v>6370029.7435195902</v>
+        <f t="shared" ref="D3:D14" si="1">($I$1*C3)/$A$1</f>
+        <v>3185014.8717343695</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3185014.8717343695</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -521,14 +522,14 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>69.295657743849219</v>
+        <v>34.647828871648024</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:F62" si="1">($I$1*C4)/$A$1</f>
-        <v>6748811.4232345019</v>
-      </c>
-      <c r="F4">
-        <v>6748811.4232345019</v>
+        <f t="shared" si="1"/>
+        <v>3374405.7115903138</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3374405.7115903138</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -538,14 +539,14 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>73.416191979009994</v>
+        <v>36.708095989211962</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="1"/>
-        <v>7150116.6337121418</v>
-      </c>
-      <c r="F5">
-        <v>7150116.6337121418</v>
+        <v>3575058.3168275319</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3575058.3168275319</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -555,14 +556,14 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>77.781745930209752</v>
+        <v>38.890872964794411</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="1"/>
-        <v>7575284.6937875729</v>
-      </c>
-      <c r="F6">
-        <v>7575284.6937875729</v>
+        <v>3787642.3468635501</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3787642.3468635501</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -572,14 +573,14 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>82.406889227943367</v>
+        <v>41.203444613642759</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="1"/>
-        <v>8025734.5623381278</v>
-      </c>
-      <c r="F7">
-        <v>8025734.5623381278</v>
+        <v>4012867.2811370296</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4012867.2811370296</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -589,14 +590,14 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>87.307057858018638</v>
+        <v>43.653528928660833</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>8502969.5739267543</v>
-      </c>
-      <c r="F8">
-        <v>8502969.5739267543</v>
+        <v>4251484.7869294379</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4251484.7869294379</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -606,14 +607,14 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>92.498605677723987</v>
+        <v>46.249302838492788</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="1"/>
-        <v>9008582.4560413696</v>
-      </c>
-      <c r="F9">
-        <v>9008582.4560413696</v>
+        <v>4504291.2279847274</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4504291.2279847274</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -623,14 +624,14 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>97.998858995306932</v>
+        <v>48.999429497262305</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="1"/>
-        <v>9544260.6446748003</v>
-      </c>
-      <c r="F10">
-        <v>9544260.6446748003</v>
+        <v>4772130.3222993044</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4772130.3222993044</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -639,15 +640,15 @@
         <v>16</v>
       </c>
       <c r="C11">
-        <f>C12/$F$1</f>
-        <v>103.82617439491722</v>
+        <f t="shared" si="0"/>
+        <v>51.913087197044185</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
-        <v>10111791.915985534</v>
-      </c>
-      <c r="F11">
-        <v>10111791.915985534</v>
+        <v>5055895.9579524053</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5055895.9579524053</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -656,14 +657,15 @@
         <v>5</v>
       </c>
       <c r="C12">
-        <v>110</v>
+        <f t="shared" si="0"/>
+        <v>54.999999999560934</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
-        <v>10713070.352834467</v>
-      </c>
-      <c r="F12">
-        <v>10713070.352834467</v>
+        <v>5356535.1763744727</v>
+      </c>
+      <c r="F12" s="1">
+        <v>5356535.1763744727</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -672,15 +674,15 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <f>C12*$F$1</f>
-        <v>116.5409403796</v>
+        <f t="shared" si="0"/>
+        <v>58.27047018933483</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
-        <v>11350102.666110381</v>
-      </c>
-      <c r="F13">
-        <v>11350102.666110381</v>
+        <v>5675051.3330098875</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5675051.3330098875</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -689,34 +691,34 @@
         <v>7</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:C62" si="2">C13*$F$1</f>
-        <v>123.4708253141953</v>
+        <f t="shared" si="0"/>
+        <v>61.735412656604815</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
-        <v>12025014.89194099</v>
-      </c>
-      <c r="F14">
-        <v>12025014.89194099</v>
+        <v>6012507.4459224977</v>
+      </c>
+      <c r="F14" s="1">
+        <v>6012507.4459224977</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
-        <v>130.81278265056037</v>
+        <f t="shared" ref="C15:C22" si="2">C16/$F$1</f>
+        <v>65.406391324758047</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
-        <v>12740059.487140883</v>
-      </c>
-      <c r="F15">
-        <v>12740059.487140883</v>
+        <f>($I$1*C15)/$A$1</f>
+        <v>6370029.7435195902</v>
+      </c>
+      <c r="F15" s="1">
+        <v>6370029.7435195902</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -726,14 +728,14 @@
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
-        <v>138.59131548880481</v>
+        <v>69.295657743849219</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>13497622.846576756</v>
-      </c>
-      <c r="F16">
-        <v>13497622.846576756</v>
+        <f t="shared" ref="D16:D79" si="3">($I$1*C16)/$A$1</f>
+        <v>6748811.4232345019</v>
+      </c>
+      <c r="F16" s="1">
+        <v>6748811.4232345019</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -742,15 +744,15 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
-        <v>146.83238395919216</v>
+        <f>C18/$F$1</f>
+        <v>73.416191979009994</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
-        <v>14300233.267538443</v>
-      </c>
-      <c r="F17">
-        <v>14300233.267538443</v>
+        <f t="shared" si="3"/>
+        <v>7150116.6337121418</v>
+      </c>
+      <c r="F17" s="1">
+        <v>7150116.6337121418</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -760,14 +762,14 @@
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>155.56349186166136</v>
+        <v>77.781745930209752</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
-        <v>15150569.387696093</v>
-      </c>
-      <c r="F18">
-        <v>15150569.387696093</v>
+        <f t="shared" si="3"/>
+        <v>7575284.6937875729</v>
+      </c>
+      <c r="F18" s="1">
+        <v>7575284.6937875729</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -777,14 +779,14 @@
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>164.81377845720243</v>
+        <v>82.406889227943367</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
-        <v>16051469.124804394</v>
-      </c>
-      <c r="F19">
-        <v>16051469.124804394</v>
+        <f t="shared" si="3"/>
+        <v>8025734.5623381278</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8025734.5623381278</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -794,14 +796,14 @@
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
-        <v>174.61411571743122</v>
+        <v>87.307057858018638</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="1"/>
-        <v>17005939.147989266</v>
-      </c>
-      <c r="F20">
-        <v>17005939.147989266</v>
+        <f t="shared" si="3"/>
+        <v>8502969.5739267543</v>
+      </c>
+      <c r="F20" s="1">
+        <v>8502969.5739267543</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -811,14 +813,14 @@
       </c>
       <c r="C21">
         <f t="shared" si="2"/>
-        <v>184.99721135692479</v>
+        <v>92.498605677723987</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="1"/>
-        <v>18017164.912226573</v>
-      </c>
-      <c r="F21">
-        <v>18017164.912226573</v>
+        <f t="shared" si="3"/>
+        <v>9008582.4560413696</v>
+      </c>
+      <c r="F21" s="1">
+        <v>9008582.4560413696</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -828,14 +830,14 @@
       </c>
       <c r="C22">
         <f t="shared" si="2"/>
-        <v>195.99771799217848</v>
+        <v>97.998858995306932</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="1"/>
-        <v>19088521.28950198</v>
-      </c>
-      <c r="F22">
-        <v>19088521.28950198</v>
+        <f t="shared" si="3"/>
+        <v>9544260.6446748003</v>
+      </c>
+      <c r="F22" s="1">
+        <v>9544260.6446748003</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -844,15 +846,15 @@
         <v>16</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
-        <v>207.65234879149207</v>
+        <f>C24/$F$1</f>
+        <v>103.82617439491722</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="1"/>
-        <v>20223583.832132507</v>
-      </c>
-      <c r="F23">
-        <v>20223583.832132507</v>
+        <f t="shared" si="3"/>
+        <v>10111791.915985534</v>
+      </c>
+      <c r="F23" s="1">
+        <v>10111791.915985534</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -861,15 +863,14 @@
         <v>5</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
-        <v>220.00000000175621</v>
+        <v>110</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="1"/>
-        <v>21426140.705839973</v>
-      </c>
-      <c r="F24">
-        <v>21426140.705839973</v>
+        <f t="shared" si="3"/>
+        <v>10713070.352834467</v>
+      </c>
+      <c r="F24" s="1">
+        <v>10713070.352834467</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -878,15 +879,15 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
-        <v>233.08188076106066</v>
+        <f>C24*$F$1</f>
+        <v>116.5409403796</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="1"/>
-        <v>22700205.332401976</v>
-      </c>
-      <c r="F25">
-        <v>22700205.332401976</v>
+        <f t="shared" si="3"/>
+        <v>11350102.666110381</v>
+      </c>
+      <c r="F25" s="1">
+        <v>11350102.666110381</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -895,34 +896,34 @@
         <v>7</v>
       </c>
       <c r="C26">
-        <f t="shared" si="2"/>
-        <v>246.94165063036189</v>
+        <f t="shared" ref="C26:C86" si="4">C25*$F$1</f>
+        <v>123.4708253141953</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>24050029.784073971</v>
-      </c>
-      <c r="F26">
-        <v>24050029.784073971</v>
+        <f t="shared" si="3"/>
+        <v>12025014.89194099</v>
+      </c>
+      <c r="F26" s="1">
+        <v>12025014.89194099</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
         <v>8</v>
       </c>
       <c r="C27">
-        <f t="shared" si="2"/>
-        <v>261.62556530320927</v>
+        <f t="shared" si="4"/>
+        <v>130.81278265056037</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="1"/>
-        <v>25480118.974485174</v>
-      </c>
-      <c r="F27">
-        <v>25480118.974485174</v>
+        <f t="shared" si="3"/>
+        <v>12740059.487140883</v>
+      </c>
+      <c r="F27" s="1">
+        <v>12740059.487140883</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -931,15 +932,15 @@
         <v>9</v>
       </c>
       <c r="C28">
-        <f t="shared" si="2"/>
-        <v>277.18263097982236</v>
+        <f t="shared" si="4"/>
+        <v>138.59131548880481</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="1"/>
-        <v>26995245.693369012</v>
-      </c>
-      <c r="F28">
-        <v>26995245.693369012</v>
+        <f t="shared" si="3"/>
+        <v>13497622.846576756</v>
+      </c>
+      <c r="F28" s="1">
+        <v>13497622.846576756</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -948,15 +949,15 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <f t="shared" si="2"/>
-        <v>293.66476792072865</v>
+        <f t="shared" si="4"/>
+        <v>146.83238395919216</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="1"/>
-        <v>28600466.535305202</v>
-      </c>
-      <c r="F29">
-        <v>28600466.535305202</v>
+        <f t="shared" si="3"/>
+        <v>14300233.267538443</v>
+      </c>
+      <c r="F29" s="1">
+        <v>14300233.267538443</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -965,15 +966,15 @@
         <v>11</v>
       </c>
       <c r="C30">
-        <f t="shared" si="2"/>
-        <v>311.12698372580644</v>
+        <f t="shared" si="4"/>
+        <v>155.56349186166136</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="1"/>
-        <v>30301138.77563408</v>
-      </c>
-      <c r="F30">
-        <v>30301138.77563408</v>
+        <f t="shared" si="3"/>
+        <v>15150569.387696093</v>
+      </c>
+      <c r="F30" s="1">
+        <v>15150569.387696093</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -982,15 +983,15 @@
         <v>12</v>
       </c>
       <c r="C31">
-        <f t="shared" si="2"/>
-        <v>329.62755691703626</v>
+        <f t="shared" si="4"/>
+        <v>164.81377845720243</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="1"/>
-        <v>32102938.249865063</v>
-      </c>
-      <c r="F31">
-        <v>32102938.249865063</v>
+        <f t="shared" si="3"/>
+        <v>16051469.124804394</v>
+      </c>
+      <c r="F31" s="1">
+        <v>16051469.124804394</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -999,15 +1000,15 @@
         <v>13</v>
       </c>
       <c r="C32">
-        <f t="shared" si="2"/>
-        <v>349.22823143765027</v>
+        <f t="shared" si="4"/>
+        <v>174.61411571743122</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="1"/>
-        <v>34011878.296250045</v>
-      </c>
-      <c r="F32">
-        <v>34011878.296250045</v>
+        <f t="shared" si="3"/>
+        <v>17005939.147989266</v>
+      </c>
+      <c r="F32" s="1">
+        <v>17005939.147989266</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1016,15 +1017,15 @@
         <v>14</v>
       </c>
       <c r="C33">
-        <f t="shared" si="2"/>
-        <v>369.99442271680323</v>
+        <f t="shared" si="4"/>
+        <v>184.99721135692479</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="1"/>
-        <v>36034329.824740805</v>
-      </c>
-      <c r="F33">
-        <v>36034329.824740805</v>
+        <f t="shared" si="3"/>
+        <v>18017164.912226573</v>
+      </c>
+      <c r="F33" s="1">
+        <v>18017164.912226573</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1033,15 +1034,15 @@
         <v>15</v>
       </c>
       <c r="C34">
-        <f t="shared" si="2"/>
-        <v>391.99543598748625</v>
+        <f t="shared" si="4"/>
+        <v>195.99771799217848</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="1"/>
-        <v>38177042.579308726</v>
-      </c>
-      <c r="F34">
-        <v>38177042.579308726</v>
+        <f t="shared" si="3"/>
+        <v>19088521.28950198</v>
+      </c>
+      <c r="F34" s="1">
+        <v>19088521.28950198</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1050,15 +1051,15 @@
         <v>16</v>
       </c>
       <c r="C35">
-        <f t="shared" si="2"/>
-        <v>415.30469758629954</v>
+        <f t="shared" si="4"/>
+        <v>207.65234879149207</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="1"/>
-        <v>40447167.664587907</v>
-      </c>
-      <c r="F35">
-        <v>40447167.664587907</v>
+        <f t="shared" si="3"/>
+        <v>20223583.832132507</v>
+      </c>
+      <c r="F35" s="1">
+        <v>20223583.832132507</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1067,15 +1068,15 @@
         <v>5</v>
       </c>
       <c r="C36">
-        <f t="shared" si="2"/>
-        <v>440.00000000702499</v>
+        <f t="shared" si="4"/>
+        <v>220.00000000175621</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="1"/>
-        <v>42852281.412022047</v>
-      </c>
-      <c r="F36">
-        <v>42852281.412022047</v>
+        <f t="shared" si="3"/>
+        <v>21426140.705839973</v>
+      </c>
+      <c r="F36" s="1">
+        <v>21426140.705839973</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1084,15 +1085,15 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <f t="shared" si="2"/>
-        <v>466.16376152584274</v>
+        <f t="shared" si="4"/>
+        <v>233.08188076106066</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="1"/>
-        <v>45400410.665166385</v>
-      </c>
-      <c r="F37">
-        <v>45400410.665166385</v>
+        <f t="shared" si="3"/>
+        <v>22700205.332401976</v>
+      </c>
+      <c r="F37" s="1">
+        <v>22700205.332401976</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1101,34 +1102,34 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <f t="shared" si="2"/>
-        <v>493.8833012646665</v>
+        <f t="shared" si="4"/>
+        <v>246.94165063036189</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="1"/>
-        <v>48100059.56853193</v>
-      </c>
-      <c r="F38">
-        <v>48100059.56853193</v>
+        <f t="shared" si="3"/>
+        <v>24050029.784073971</v>
+      </c>
+      <c r="F38" s="1">
+        <v>24050029.784073971</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
         <v>8</v>
       </c>
       <c r="C39">
-        <f t="shared" si="2"/>
-        <v>523.25113061059574</v>
+        <f t="shared" si="4"/>
+        <v>261.62556530320927</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="1"/>
-        <v>50960237.949377172</v>
-      </c>
-      <c r="F39">
-        <v>50960237.949377172</v>
+        <f t="shared" si="3"/>
+        <v>25480118.974485174</v>
+      </c>
+      <c r="F39" s="1">
+        <v>25480118.974485174</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1137,15 +1138,15 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <f t="shared" si="2"/>
-        <v>554.36526196407033</v>
+        <f t="shared" si="4"/>
+        <v>277.18263097982236</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="1"/>
-        <v>53990491.387169041</v>
-      </c>
-      <c r="F40">
-        <v>53990491.387169041</v>
+        <f t="shared" si="3"/>
+        <v>26995245.693369012</v>
+      </c>
+      <c r="F40" s="1">
+        <v>26995245.693369012</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1154,15 +1155,15 @@
         <v>10</v>
       </c>
       <c r="C41">
-        <f t="shared" si="2"/>
-        <v>587.32953584614597</v>
+        <f t="shared" si="4"/>
+        <v>293.66476792072865</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="1"/>
-        <v>57200933.071067043</v>
-      </c>
-      <c r="F41">
-        <v>57200933.071067043</v>
+        <f t="shared" si="3"/>
+        <v>28600466.535305202</v>
+      </c>
+      <c r="F41" s="1">
+        <v>28600466.535305202</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1171,15 +1172,15 @@
         <v>11</v>
       </c>
       <c r="C42">
-        <f t="shared" si="2"/>
-        <v>622.25396745658043</v>
+        <f t="shared" si="4"/>
+        <v>311.12698372580644</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="1"/>
-        <v>60602277.551751956</v>
-      </c>
-      <c r="F42">
-        <v>60602277.551751956</v>
+        <f t="shared" si="3"/>
+        <v>30301138.77563408</v>
+      </c>
+      <c r="F42" s="1">
+        <v>30301138.77563408</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1188,15 +1189,15 @@
         <v>12</v>
       </c>
       <c r="C43">
-        <f t="shared" si="2"/>
-        <v>659.25511383933554</v>
+        <f t="shared" si="4"/>
+        <v>329.62755691703626</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="1"/>
-        <v>64205876.500242703</v>
-      </c>
-      <c r="F43">
-        <v>64205876.500242703</v>
+        <f t="shared" si="3"/>
+        <v>32102938.249865063</v>
+      </c>
+      <c r="F43" s="1">
+        <v>32102938.249865063</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1205,15 +1206,15 @@
         <v>13</v>
       </c>
       <c r="C44">
-        <f t="shared" si="2"/>
-        <v>698.45646288087653</v>
+        <f t="shared" si="4"/>
+        <v>349.22823143765027</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="1"/>
-        <v>68023756.593043149</v>
-      </c>
-      <c r="F44">
-        <v>68023756.593043149</v>
+        <f t="shared" si="3"/>
+        <v>34011878.296250045</v>
+      </c>
+      <c r="F44" s="1">
+        <v>34011878.296250045</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1222,15 +1223,15 @@
         <v>14</v>
       </c>
       <c r="C45">
-        <f t="shared" si="2"/>
-        <v>739.98884543951397</v>
+        <f t="shared" si="4"/>
+        <v>369.99442271680323</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="1"/>
-        <v>72068659.650056943</v>
-      </c>
-      <c r="F45">
-        <v>72068659.650056943</v>
+        <f t="shared" si="3"/>
+        <v>36034329.824740805</v>
+      </c>
+      <c r="F45" s="1">
+        <v>36034329.824740805</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1239,15 +1240,15 @@
         <v>15</v>
       </c>
       <c r="C46">
-        <f t="shared" si="2"/>
-        <v>783.99087198123129</v>
+        <f t="shared" si="4"/>
+        <v>391.99543598748625</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="1"/>
-        <v>76354085.159227014</v>
-      </c>
-      <c r="F46">
-        <v>76354085.159227014</v>
+        <f t="shared" si="3"/>
+        <v>38177042.579308726</v>
+      </c>
+      <c r="F46" s="1">
+        <v>38177042.579308726</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1256,15 +1257,15 @@
         <v>16</v>
       </c>
       <c r="C47">
-        <f t="shared" si="2"/>
-        <v>830.60939517922998</v>
+        <f t="shared" si="4"/>
+        <v>415.30469758629954</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="1"/>
-        <v>80894335.329821602</v>
-      </c>
-      <c r="F47">
-        <v>80894335.329821602</v>
+        <f t="shared" si="3"/>
+        <v>40447167.664587907</v>
+      </c>
+      <c r="F47" s="1">
+        <v>40447167.664587907</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1273,15 +1274,15 @@
         <v>5</v>
       </c>
       <c r="C48">
-        <f t="shared" si="2"/>
-        <v>880.00000002107515</v>
+        <f t="shared" si="4"/>
+        <v>440.00000000702499</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="1"/>
-        <v>85704562.82472828</v>
-      </c>
-      <c r="F48">
-        <v>85704562.82472828</v>
+        <f t="shared" si="3"/>
+        <v>42852281.412022047</v>
+      </c>
+      <c r="F48" s="1">
+        <v>42852281.412022047</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1290,15 +1291,15 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <f t="shared" si="2"/>
-        <v>932.32752305912845</v>
+        <f t="shared" si="4"/>
+        <v>466.16376152584274</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="1"/>
-        <v>90800821.331057653</v>
-      </c>
-      <c r="F49">
-        <v>90800821.331057653</v>
+        <f t="shared" si="3"/>
+        <v>45400410.665166385</v>
+      </c>
+      <c r="F49" s="1">
+        <v>45400410.665166385</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1307,34 +1308,34 @@
         <v>7</v>
       </c>
       <c r="C50">
-        <f t="shared" si="2"/>
-        <v>987.76660253721855</v>
+        <f t="shared" si="4"/>
+        <v>493.8833012646665</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="1"/>
-        <v>96200119.137831837</v>
-      </c>
-      <c r="F50">
-        <v>96200119.137831837</v>
+        <f t="shared" si="3"/>
+        <v>48100059.56853193</v>
+      </c>
+      <c r="F50" s="1">
+        <v>48100059.56853193</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
         <v>8</v>
       </c>
       <c r="C51">
-        <f t="shared" si="2"/>
-        <v>1046.5022612295459</v>
+        <f t="shared" si="4"/>
+        <v>523.25113061059574</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="1"/>
-        <v>101920475.89956799</v>
-      </c>
-      <c r="F51">
-        <v>101920475.89956799</v>
+        <f t="shared" si="3"/>
+        <v>50960237.949377172</v>
+      </c>
+      <c r="F51" s="1">
+        <v>50960237.949377172</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1343,15 +1344,15 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <f t="shared" si="2"/>
-        <v>1108.7305239369919</v>
+        <f t="shared" si="4"/>
+        <v>554.36526196407033</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="1"/>
-        <v>107980982.77520011</v>
-      </c>
-      <c r="F52">
-        <v>107980982.77520011</v>
+        <f t="shared" si="3"/>
+        <v>53990491.387169041</v>
+      </c>
+      <c r="F52" s="1">
+        <v>53990491.387169041</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1360,15 +1361,15 @@
         <v>10</v>
       </c>
       <c r="C53">
-        <f t="shared" si="2"/>
-        <v>1174.6590717016695</v>
+        <f t="shared" si="4"/>
+        <v>587.32953584614597</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="1"/>
-        <v>114401866.14304738</v>
-      </c>
-      <c r="F53">
-        <v>114401866.14304738</v>
+        <f t="shared" si="3"/>
+        <v>57200933.071067043</v>
+      </c>
+      <c r="F53" s="1">
+        <v>57200933.071067043</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1377,15 +1378,15 @@
         <v>11</v>
       </c>
       <c r="C54">
-        <f t="shared" si="2"/>
-        <v>1244.5079349230959</v>
+        <f t="shared" si="4"/>
+        <v>622.25396745658043</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="1"/>
-        <v>121204555.1044715</v>
-      </c>
-      <c r="F54">
-        <v>121204555.1044715</v>
+        <f t="shared" si="3"/>
+        <v>60602277.551751956</v>
+      </c>
+      <c r="F54" s="1">
+        <v>60602277.551751956</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1394,15 +1395,15 @@
         <v>12</v>
       </c>
       <c r="C55">
-        <f t="shared" si="2"/>
-        <v>1318.5102276891969</v>
+        <f t="shared" si="4"/>
+        <v>659.25511383933554</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="1"/>
-        <v>128411753.00151053</v>
-      </c>
-      <c r="F55">
-        <v>128411753.00151053</v>
+        <f t="shared" si="3"/>
+        <v>64205876.500242703</v>
+      </c>
+      <c r="F55" s="1">
+        <v>64205876.500242703</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1411,15 +1412,15 @@
         <v>13</v>
       </c>
       <c r="C56">
-        <f t="shared" si="2"/>
-        <v>1396.9129257729048</v>
+        <f t="shared" si="4"/>
+        <v>698.45646288087653</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="1"/>
-        <v>136047513.18717238</v>
-      </c>
-      <c r="F56">
-        <v>136047513.18717238</v>
+        <f t="shared" si="3"/>
+        <v>68023756.593043149</v>
+      </c>
+      <c r="F56" s="1">
+        <v>68023756.593043149</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1428,15 +1429,15 @@
         <v>14</v>
       </c>
       <c r="C57">
-        <f t="shared" si="2"/>
-        <v>1479.977690890843</v>
+        <f t="shared" si="4"/>
+        <v>739.98884543951397</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="1"/>
-        <v>144137319.30126458</v>
-      </c>
-      <c r="F57">
-        <v>144137319.30126458</v>
+        <f t="shared" si="3"/>
+        <v>72068659.650056943</v>
+      </c>
+      <c r="F57" s="1">
+        <v>72068659.650056943</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1445,15 +1446,15 @@
         <v>15</v>
       </c>
       <c r="C58">
-        <f t="shared" si="2"/>
-        <v>1567.9817439749802</v>
+        <f t="shared" si="4"/>
+        <v>783.99087198123129</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="1"/>
-        <v>152708170.31967312</v>
-      </c>
-      <c r="F58">
-        <v>152708170.31967312</v>
+        <f t="shared" si="3"/>
+        <v>76354085.159227014</v>
+      </c>
+      <c r="F58" s="1">
+        <v>76354085.159227014</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1462,15 +1463,15 @@
         <v>16</v>
       </c>
       <c r="C59">
-        <f t="shared" si="2"/>
-        <v>1661.218790371722</v>
+        <f t="shared" si="4"/>
+        <v>830.60939517922998</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="1"/>
-        <v>161788670.66093481</v>
-      </c>
-      <c r="F59">
-        <v>161788670.66093481</v>
+        <f t="shared" si="3"/>
+        <v>80894335.329821602</v>
+      </c>
+      <c r="F59" s="1">
+        <v>80894335.329821602</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1479,15 +1480,15 @@
         <v>5</v>
       </c>
       <c r="C60">
-        <f t="shared" si="2"/>
-        <v>1760.0000000562009</v>
+        <f t="shared" si="4"/>
+        <v>880.00000002107515</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="1"/>
-        <v>171409125.65082496</v>
-      </c>
-      <c r="F60">
-        <v>171409125.65082496</v>
+        <f t="shared" si="3"/>
+        <v>85704562.82472828</v>
+      </c>
+      <c r="F60" s="1">
+        <v>85704562.82472828</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1496,15 +1497,15 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <f t="shared" si="2"/>
-        <v>1864.6550461331428</v>
+        <f t="shared" si="4"/>
+        <v>932.32752305912845</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="1"/>
-        <v>181601642.66356507</v>
-      </c>
-      <c r="F61">
-        <v>181601642.66356507</v>
+        <f t="shared" si="3"/>
+        <v>90800821.331057653</v>
+      </c>
+      <c r="F61" s="1">
+        <v>90800821.331057653</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -1513,24 +1514,438 @@
         <v>7</v>
       </c>
       <c r="C62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
+        <v>987.76660253721855</v>
+      </c>
+      <c r="D62" s="1">
+        <f t="shared" si="3"/>
+        <v>96200119.137831837</v>
+      </c>
+      <c r="F62" s="1">
+        <v>96200119.137831837</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="2">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="4"/>
+        <v>1046.5022612295459</v>
+      </c>
+      <c r="D63" s="1">
+        <f t="shared" si="3"/>
+        <v>101920475.89956799</v>
+      </c>
+      <c r="F63" s="1">
+        <v>101920475.89956799</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A64" s="2"/>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="4"/>
+        <v>1108.7305239369919</v>
+      </c>
+      <c r="D64" s="1">
+        <f t="shared" si="3"/>
+        <v>107980982.77520011</v>
+      </c>
+      <c r="F64" s="1">
+        <v>107980982.77520011</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A65" s="2"/>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="4"/>
+        <v>1174.6590717016695</v>
+      </c>
+      <c r="D65" s="1">
+        <f t="shared" si="3"/>
+        <v>114401866.14304738</v>
+      </c>
+      <c r="F65" s="1">
+        <v>114401866.14304738</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A66" s="2"/>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="4"/>
+        <v>1244.5079349230959</v>
+      </c>
+      <c r="D66" s="1">
+        <f t="shared" si="3"/>
+        <v>121204555.1044715</v>
+      </c>
+      <c r="F66" s="1">
+        <v>121204555.1044715</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A67" s="2"/>
+      <c r="B67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="4"/>
+        <v>1318.5102276891969</v>
+      </c>
+      <c r="D67" s="1">
+        <f t="shared" si="3"/>
+        <v>128411753.00151053</v>
+      </c>
+      <c r="F67" s="1">
+        <v>128411753.00151053</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A68" s="2"/>
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="4"/>
+        <v>1396.9129257729048</v>
+      </c>
+      <c r="D68" s="1">
+        <f t="shared" si="3"/>
+        <v>136047513.18717238</v>
+      </c>
+      <c r="F68" s="1">
+        <v>136047513.18717238</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="2"/>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="4"/>
+        <v>1479.977690890843</v>
+      </c>
+      <c r="D69" s="1">
+        <f t="shared" si="3"/>
+        <v>144137319.30126458</v>
+      </c>
+      <c r="F69" s="1">
+        <v>144137319.30126458</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A70" s="2"/>
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="4"/>
+        <v>1567.9817439749802</v>
+      </c>
+      <c r="D70" s="1">
+        <f t="shared" si="3"/>
+        <v>152708170.31967312</v>
+      </c>
+      <c r="F70" s="1">
+        <v>152708170.31967312</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A71" s="2"/>
+      <c r="B71" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="4"/>
+        <v>1661.218790371722</v>
+      </c>
+      <c r="D71" s="1">
+        <f t="shared" si="3"/>
+        <v>161788670.66093481</v>
+      </c>
+      <c r="F71" s="1">
+        <v>161788670.66093481</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A72" s="2"/>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="4"/>
+        <v>1760.0000000562009</v>
+      </c>
+      <c r="D72" s="1">
+        <f t="shared" si="3"/>
+        <v>171409125.65082496</v>
+      </c>
+      <c r="F72" s="1">
+        <v>171409125.65082496</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A73" s="2"/>
+      <c r="B73" t="s">
+        <v>6</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="4"/>
+        <v>1864.6550461331428</v>
+      </c>
+      <c r="D73" s="1">
+        <f t="shared" si="3"/>
+        <v>181601642.66356507</v>
+      </c>
+      <c r="F73" s="1">
+        <v>181601642.66356507</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A74" s="2"/>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="4"/>
         <v>1975.5332050902082</v>
       </c>
-      <c r="D62" s="1">
-        <f t="shared" si="1"/>
+      <c r="D74" s="1">
+        <f t="shared" si="3"/>
         <v>192400238.27719966</v>
       </c>
-      <c r="F62">
+      <c r="F74" s="1">
         <v>192400238.27719966</v>
       </c>
     </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A75" s="2">
+        <v>7</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="4"/>
+        <v>2093.0045224758005</v>
+      </c>
+      <c r="D75" s="1">
+        <f t="shared" si="3"/>
+        <v>203840951.80076328</v>
+      </c>
+      <c r="F75" s="1">
+        <v>203840951.80076328</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A76" s="2"/>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="4"/>
+        <v>2217.4610478916861</v>
+      </c>
+      <c r="D76" s="1">
+        <f t="shared" si="3"/>
+        <v>215961965.55212429</v>
+      </c>
+      <c r="F76" s="1">
+        <v>215961965.55212429</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A77" s="2"/>
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="4"/>
+        <v>2349.3181434220942</v>
+      </c>
+      <c r="D77" s="1">
+        <f t="shared" si="3"/>
+        <v>228803732.28792137</v>
+      </c>
+      <c r="F77" s="1">
+        <v>228803732.28792137</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A78" s="2"/>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="4"/>
+        <v>2489.0158698660625</v>
+      </c>
+      <c r="D78" s="1">
+        <f t="shared" si="3"/>
+        <v>242409110.21087825</v>
+      </c>
+      <c r="F78" s="1">
+        <v>242409110.21087825</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A79" s="2"/>
+      <c r="B79" t="s">
+        <v>12</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="4"/>
+        <v>2637.0204553994458</v>
+      </c>
+      <c r="D79" s="1">
+        <f t="shared" si="3"/>
+        <v>256823506.00507134</v>
+      </c>
+      <c r="F79" s="1">
+        <v>256823506.00507134</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A80" s="2"/>
+      <c r="B80" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="4"/>
+        <v>2793.8258515681136</v>
+      </c>
+      <c r="D80" s="1">
+        <f t="shared" ref="D80:D86" si="5">($I$1*C80)/$A$1</f>
+        <v>272095026.376517</v>
+      </c>
+      <c r="F80" s="1">
+        <v>272095026.376517</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A81" s="2"/>
+      <c r="B81" t="s">
+        <v>14</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="4"/>
+        <v>2959.9553818053159</v>
+      </c>
+      <c r="D81" s="1">
+        <f t="shared" si="5"/>
+        <v>288274638.6048305</v>
+      </c>
+      <c r="F81" s="1">
+        <v>288274638.6048305</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A82" s="2"/>
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="4"/>
+        <v>3135.9634879749956</v>
+      </c>
+      <c r="D82" s="1">
+        <f t="shared" si="5"/>
+        <v>305416340.64178449</v>
+      </c>
+      <c r="F82" s="1">
+        <v>305416340.64178449</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A83" s="2"/>
+      <c r="B83" t="s">
+        <v>16</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="4"/>
+        <v>3322.4375807699676</v>
+      </c>
+      <c r="D83" s="1">
+        <f t="shared" si="5"/>
+        <v>323577341.32445282</v>
+      </c>
+      <c r="F83" s="1">
+        <v>323577341.32445282</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A84" s="2"/>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="4"/>
+        <v>3520.0000001405024</v>
+      </c>
+      <c r="D84" s="1">
+        <f t="shared" si="5"/>
+        <v>342818251.30438668</v>
+      </c>
+      <c r="F84" s="1">
+        <v>342818251.30438668</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A85" s="2"/>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="4"/>
+        <v>3729.3100922960575</v>
+      </c>
+      <c r="D85" s="1">
+        <f t="shared" si="5"/>
+        <v>363203285.33002967</v>
+      </c>
+      <c r="F85" s="1">
+        <v>363203285.33002967</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A86" s="2"/>
+      <c r="B86" t="s">
+        <v>7</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="4"/>
+        <v>3951.0664102119586</v>
+      </c>
+      <c r="D86" s="1">
+        <f t="shared" si="5"/>
+        <v>384800476.55747128</v>
+      </c>
+      <c r="F86" s="1">
+        <v>384800476.55747128</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A75:A86"/>
     <mergeCell ref="A15:A26"/>
     <mergeCell ref="A27:A38"/>
     <mergeCell ref="A39:A50"/>
     <mergeCell ref="A51:A62"/>
+    <mergeCell ref="A63:A74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>